<commit_message>
updated files to include evaporation equations of Fe3O4 and Fe
</commit_message>
<xml_diff>
--- a/test_wang_data.xlsx
+++ b/test_wang_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owen\Code\micrometeorites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8390088-53AF-4841-A297-D85CC563A6A0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B083A3-2B17-4B91-B0C7-687A8E329008}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_wang_data" sheetId="1" r:id="rId1"/>
+    <sheet name="wustite data" sheetId="1" r:id="rId1"/>
+    <sheet name="iron data" sheetId="3" r:id="rId2"/>
+    <sheet name="magnetite data" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>10000/T</t>
   </si>
@@ -44,13 +46,19 @@
     <t>J [mol m-2 s-1]</t>
   </si>
   <si>
-    <t>p [Pa] - from Wang</t>
-  </si>
-  <si>
     <t>p from fit [Pa]</t>
   </si>
   <si>
     <t>p from Genge</t>
+  </si>
+  <si>
+    <t>p [Pa] from Wang 1994</t>
+  </si>
+  <si>
+    <t>Temperature [K]</t>
+  </si>
+  <si>
+    <t>p [Pa] from fit</t>
   </si>
 </sst>
 </file>
@@ -534,9 +542,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -630,11 +639,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Fitting the Wang Data</a:t>
+              <a:t>Wang Data vs Temp</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40949300087489071"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -675,7 +692,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -695,59 +714,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.28298184429614126"/>
-                  <c:y val="1.7048611111111112E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>test_wang_data!$D$2:$D$8</c:f>
+              <c:f>'wustite data'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -777,30 +746,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>test_wang_data!$G$2:$G$8</c:f>
+              <c:f>'wustite data'!$F$2:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.6255523109999999</c:v>
+                  <c:v>4.619319366638841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4062136670000001</c:v>
+                  <c:v>1.4043187886526931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40263956000000001</c:v>
+                  <c:v>0.40209700181720415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9811995000000006E-2</c:v>
+                  <c:v>8.969097341653455E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5158487999999997E-2</c:v>
+                  <c:v>4.5097636853446005E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6628571000000002E-2</c:v>
+                  <c:v>1.66061641682777E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5186269999999999E-3</c:v>
+                  <c:v>6.5098428008912813E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,7 +777,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C704-4D21-B5D0-2AACD4791BE7}"/>
+              <c16:uniqueId val="{00000000-62E8-47E2-A074-A176C22D89D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -820,11 +789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1744717743"/>
-        <c:axId val="1736600095"/>
+        <c:axId val="676236303"/>
+        <c:axId val="556011375"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1744717743"/>
+        <c:axId val="676236303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,12 +850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1736600095"/>
+        <c:crossAx val="556011375"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1736600095"/>
+        <c:axId val="556011375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +875,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -943,7 +912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1744717743"/>
+        <c:crossAx val="676236303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -957,13 +926,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1560,22 +1522,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>633411</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1142999</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B72060A5-CD9A-4B0F-82F3-76980E5A6467}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26B1621-CA8A-4C44-9329-B71357F02D9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,6 +1553,96 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A62BD5E-73B9-4B3F-93A7-1A02D061B209}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="2314575"/>
+          <a:ext cx="2295525" cy="1628775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NOTE: this data was collected</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> using figure 1 in Wang 1994. The tool at the website:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>https://apps.automeris.io/wpd/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>was used to find the data points </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1893,23 +1945,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="43.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1920,10 +1971,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1931,11 +1982,8 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.8415272729999996</v>
       </c>
@@ -1946,24 +1994,23 @@
         <v>2065.463941</v>
       </c>
       <c r="E2" s="1">
-        <v>5.2499999999999997E-6</v>
-      </c>
-      <c r="F2">
-        <v>5.2480746000000002E-2</v>
+        <f>10^(B2)*10000</f>
+        <v>5.2480746024977203E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>E2*SQRT(2*PI()*0.0718*8.31446*D2)</f>
+        <v>4.619319366638841</v>
       </c>
       <c r="G2">
-        <v>4.6255523109999999</v>
+        <f>EXP(25.93 - 50390/D2)</f>
+        <v>4.6345730277245742</v>
       </c>
       <c r="H2">
-        <f>EXP(LN(10^-13)+0.0152*D2)</f>
-        <v>4.31218913135978</v>
-      </c>
-      <c r="I2">
         <f>10^(11.3-2.0126*10^4/D2)</f>
         <v>35.970146950464866</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.080115825</v>
       </c>
@@ -1974,24 +2021,23 @@
         <v>1968.4590559999999</v>
       </c>
       <c r="E3" s="1">
-        <v>1.6300000000000001E-6</v>
-      </c>
-      <c r="F3">
-        <v>1.6343058000000001E-2</v>
+        <f t="shared" ref="E3:E8" si="0">10^(B3)*10000</f>
+        <v>1.634305841468757E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F8" si="1">E3*SQRT(2*PI()*0.0718*8.31446*D3)</f>
+        <v>1.4043187886526931</v>
       </c>
       <c r="G3">
-        <v>1.4062136670000001</v>
+        <f t="shared" ref="G3:G8" si="2">EXP(25.93 - 50390/D3)</f>
+        <v>1.3927724946351798</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="0">EXP(LN(10^-13)+0.0152*D3)</f>
-        <v>0.98705594654788242</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I8" si="1">10^(11.3-2.0126*10^4/D3)</f>
+        <f t="shared" ref="H3:H8" si="3">10^(11.3-2.0126*10^4/D3)</f>
         <v>11.905808474181356</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.3146747469999998</v>
       </c>
@@ -2002,24 +2048,23 @@
         <v>1881.5826890000001</v>
       </c>
       <c r="E4" s="1">
-        <v>4.7899999999999999E-7</v>
-      </c>
-      <c r="F4">
-        <v>4.7863009999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.7863009232263741E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40209700181720415</v>
       </c>
       <c r="G4">
-        <v>0.40263956000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.4271388915071529</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0.26354020654756266</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.0150005205477921</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.6058424240000004</v>
       </c>
@@ -2030,24 +2075,23 @@
         <v>1783.8532090000001</v>
       </c>
       <c r="E5" s="1">
-        <v>1.1000000000000001E-7</v>
-      </c>
-      <c r="F5">
-        <v>1.0964779999999999E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.0964781961431838E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>8.969097341653455E-2</v>
       </c>
       <c r="G5">
-        <v>8.9811995000000006E-2</v>
+        <f t="shared" si="2"/>
+        <v>9.8486087696128558E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>5.9663345097108966E-2</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0415533840548161</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.7433346800000002</v>
       </c>
@@ -2058,24 +2102,23 @@
         <v>1741.1487500000001</v>
       </c>
       <c r="E6" s="1">
-        <v>5.5799999999999997E-8</v>
-      </c>
-      <c r="F6">
-        <v>5.5804200000000002E-4</v>
+        <f t="shared" si="0"/>
+        <v>5.5804171790530888E-4</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5097636853446005E-2</v>
       </c>
       <c r="G6">
-        <v>4.5158487999999997E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.9258986763046561E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>3.1174799810175881E-2</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.55076282868306725</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.9374464649999998</v>
       </c>
@@ -2086,24 +2129,23 @@
         <v>1684.2257119999999</v>
       </c>
       <c r="E7" s="1">
-        <v>2.0899999999999999E-8</v>
-      </c>
-      <c r="F7">
-        <v>2.0892999999999999E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.0892961308540368E-4</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.66061641682777E-2</v>
       </c>
       <c r="G7">
-        <v>1.6628571000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.852206162332944E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>1.3123176853896889E-2</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22402435959856551</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.1234666669999998</v>
       </c>
@@ -2114,20 +2156,19 @@
         <v>1633.061882</v>
       </c>
       <c r="E8" s="1">
-        <v>8.3199999999999994E-9</v>
+        <f t="shared" si="0"/>
+        <v>8.3176377110267023E-5</v>
       </c>
       <c r="F8" s="1">
-        <v>8.3200000000000003E-5</v>
+        <f t="shared" si="1"/>
+        <v>6.5098428008912813E-3</v>
       </c>
       <c r="G8">
-        <v>6.5186269999999999E-3</v>
+        <f t="shared" si="2"/>
+        <v>7.2543895633021714E-3</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>6.029654284205088E-3</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.4604323713669669E-2</v>
       </c>
     </row>
@@ -2136,4 +2177,353 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16C6AB9-8B80-425A-BD7D-82836A637DC5}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.7813596629142801</v>
+      </c>
+      <c r="B2" s="2">
+        <f>1/A2*10000</f>
+        <v>2091.4552982832743</v>
+      </c>
+      <c r="C2">
+        <v>1.6775342826330701E-4</v>
+      </c>
+      <c r="D2">
+        <f>10000*C2</f>
+        <v>1.6775342826330701</v>
+      </c>
+      <c r="E2">
+        <f>D2*SQRT(2*PI()*0.055845*8.31446*B2)</f>
+        <v>131.03726006585563</v>
+      </c>
+      <c r="F2">
+        <f>EXP(26.5-45210/B2)</f>
+        <v>132.08860718813861</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.0217623330069001</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B7" si="0">1/A3*10000</f>
+        <v>1991.3327905369549</v>
+      </c>
+      <c r="C3">
+        <v>5.81948440370619E-5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="1">10000*C3</f>
+        <v>0.58194844037061899</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="2">D3*SQRT(2*PI()*0.055845*8.31446*B3)</f>
+        <v>44.356322984295332</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="3">EXP(26.5-45210/B3)</f>
+        <v>44.550015082805274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.2843738489043801</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>1892.3717900983331</v>
+      </c>
+      <c r="C4">
+        <v>1.7944560104565599E-5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0.17944560104565599</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>13.333223376707162</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>13.590157657692417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.5731157968501499</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>1794.3284088322489</v>
+      </c>
+      <c r="C5">
+        <v>4.9190779995484796E-6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4.9190779995484796E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>3.5590474781220718</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>3.6837950428522164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.89974395141365</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>1694.9888134728083</v>
+      </c>
+      <c r="C6">
+        <v>1.10808969085993E-6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.10808969085993E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.77921524108358475</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>0.84135431615219503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.2211478163996796</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>1607.4204142262654</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.5963215972181998E-7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.5963215972181998E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.17779614149400005</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>0.19675238339310983</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AD3BA8-CAEB-4779-8B2B-E2DA7E5366CE}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.0276011726510399</v>
+      </c>
+      <c r="B2">
+        <f>1/A2*10000</f>
+        <v>1989.0201423290359</v>
+      </c>
+      <c r="C2">
+        <v>1.0980839744828899E-6</v>
+      </c>
+      <c r="D2">
+        <f>C2*10000</f>
+        <v>1.0980839744828899E-2</v>
+      </c>
+      <c r="E2">
+        <f>D2*SQRT(2*PI()*0.2315*8.31446*B2)</f>
+        <v>1.7030900044415427</v>
+      </c>
+      <c r="F2">
+        <f>EXP(27.74-54120/B2)</f>
+        <v>1.6999901443642464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5.2913351617569901</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B6" si="0">1/A3*10000</f>
+        <v>1889.8821742147015</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.7032718289184597E-7</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="1">C3*10000</f>
+        <v>2.7032718289184596E-3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="2">D3*SQRT(2*PI()*0.2315*8.31446*B3)</f>
+        <v>0.40868579131143623</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="3">EXP(27.74-54120/B3)</f>
+        <v>0.4079111510084496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5.5811860604819703</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1791.7338522013792</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.9119878129203802E-8</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>5.9119878129203804E-4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>8.7026744095048639E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>8.4976633581180683E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.9049790421249897</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1693.4861120864132</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.0612334302997301E-8</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1.0612334302997301E-4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>1.5187426813244984E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>1.4731804130800984E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6.2170252641952199</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1608.4863057564683</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.0616295558676399E-9</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.06162955586764E-5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>2.8754231942910609E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>2.7215853210849385E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating model to use O stoichiometry
</commit_message>
<xml_diff>
--- a/test_wang_data.xlsx
+++ b/test_wang_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owen\Code\micrometeorites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B083A3-2B17-4B91-B0C7-687A8E329008}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3F8E7F-4914-481F-A5F2-7D9CFD05B8CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wustite data" sheetId="1" r:id="rId1"/>
     <sheet name="iron data" sheetId="3" r:id="rId2"/>
     <sheet name="magnetite data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>10000/T</t>
   </si>
@@ -49,9 +49,6 @@
     <t>p from fit [Pa]</t>
   </si>
   <si>
-    <t>p from Genge</t>
-  </si>
-  <si>
     <t>p [Pa] from Wang 1994</t>
   </si>
   <si>
@@ -59,6 +56,12 @@
   </si>
   <si>
     <t>p [Pa] from fit</t>
+  </si>
+  <si>
+    <t>p from Genge [dynes cm-2]</t>
+  </si>
+  <si>
+    <t>p from Genge [Pa]</t>
   </si>
 </sst>
 </file>
@@ -1945,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,10 +1960,11 @@
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1974,16 +1978,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.8415272729999996</v>
       </c>
@@ -2009,8 +2016,12 @@
         <f>10^(11.3-2.0126*10^4/D2)</f>
         <v>35.970146950464866</v>
       </c>
+      <c r="I2">
+        <f>10^((11.3-2.0126*10^4/D2)-1)</f>
+        <v>3.5970146950464863</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.080115825</v>
       </c>
@@ -2036,8 +2047,12 @@
         <f t="shared" ref="H3:H8" si="3">10^(11.3-2.0126*10^4/D3)</f>
         <v>11.905808474181356</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="4">10^((11.3-2.0126*10^4/D3)-1)</f>
+        <v>1.1905808474181356</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.3146747469999998</v>
       </c>
@@ -2063,8 +2078,12 @@
         <f t="shared" si="3"/>
         <v>4.0150005205477921</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>0.40150005205477912</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.6058424240000004</v>
       </c>
@@ -2090,8 +2109,12 @@
         <f t="shared" si="3"/>
         <v>1.0415533840548161</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>0.10415533840548159</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.7433346800000002</v>
       </c>
@@ -2117,8 +2140,12 @@
         <f t="shared" si="3"/>
         <v>0.55076282868306725</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>5.5076282868306722E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.9374464649999998</v>
       </c>
@@ -2144,8 +2171,12 @@
         <f t="shared" si="3"/>
         <v>0.22402435959856551</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>2.2402435959856543E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.1234666669999998</v>
       </c>
@@ -2170,6 +2201,10 @@
       <c r="H8">
         <f t="shared" si="3"/>
         <v>9.4604323713669669E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>9.460432371366961E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16C6AB9-8B80-425A-BD7D-82836A637DC5}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2201,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -2210,10 +2245,10 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2371,7 +2406,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,10 +2432,10 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new filename (again) with dynamic ODE solver!
</commit_message>
<xml_diff>
--- a/test_wang_data.xlsx
+++ b/test_wang_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owen\Code\micrometeorites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3F8E7F-4914-481F-A5F2-7D9CFD05B8CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF4C2CC-F735-4E91-91AF-F6889FF4CB4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="1125" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wustite data" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>10000/T</t>
   </si>
@@ -62,6 +63,12 @@
   </si>
   <si>
     <t>p from Genge [Pa]</t>
+  </si>
+  <si>
+    <t>Genge pressure with natural log [dynes cm-2]</t>
+  </si>
+  <si>
+    <t>base 10 fit [Pa]</t>
   </si>
 </sst>
 </file>
@@ -545,10 +552,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1530,7 +1536,7 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1948,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,12 +1965,12 @@
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="7" max="8" width="34.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1984,13 +1990,16 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.8415272729999996</v>
       </c>
@@ -2013,15 +2022,19 @@
         <v>4.6345730277245742</v>
       </c>
       <c r="H2">
+        <f>EXP(11.3-2.0126*10^4/D2)</f>
+        <v>4.7395500832911193</v>
+      </c>
+      <c r="I2">
         <f>10^(11.3-2.0126*10^4/D2)</f>
         <v>35.970146950464866</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>10^((11.3-2.0126*10^4/D2)-1)</f>
         <v>3.5970146950464863</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.080115825</v>
       </c>
@@ -2044,15 +2057,19 @@
         <v>1.3927724946351798</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="3">10^(11.3-2.0126*10^4/D3)</f>
+        <f t="shared" ref="H3:H8" si="3">EXP(11.3-2.0126*10^4/D3)</f>
+        <v>2.9322172922934069</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="4">10^(11.3-2.0126*10^4/D3)</f>
         <v>11.905808474181356</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I8" si="4">10^((11.3-2.0126*10^4/D3)-1)</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="5">10^((11.3-2.0126*10^4/D3)-1)</f>
         <v>1.1905808474181356</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.3146747469999998</v>
       </c>
@@ -2076,14 +2093,18 @@
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>4.0150005205477921</v>
+        <v>1.8288468029977487</v>
       </c>
       <c r="I4">
         <f t="shared" si="4"/>
+        <v>4.0150005205477921</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="5"/>
         <v>0.40150005205477912</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.6058424240000004</v>
       </c>
@@ -2107,14 +2128,18 @@
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>1.0415533840548161</v>
+        <v>1.0178387780299463</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
+        <v>1.0415533840548161</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
         <v>0.10415533840548159</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.7433346800000002</v>
       </c>
@@ -2138,14 +2163,18 @@
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>0.55076282868306725</v>
+        <v>0.77179571779913458</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
+        <v>0.55076282868306725</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
         <v>5.5076282868306722E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.9374464649999998</v>
       </c>
@@ -2169,14 +2198,18 @@
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>0.22402435959856551</v>
+        <v>0.52219993066752979</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
+        <v>0.22402435959856551</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
         <v>2.2402435959856543E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6.1234666669999998</v>
       </c>
@@ -2200,10 +2233,14 @@
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>9.4604323713669669E-2</v>
+        <v>0.35912347270030981</v>
       </c>
       <c r="I8">
         <f t="shared" si="4"/>
+        <v>9.4604323713669669E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
         <v>9.460432371366961E-3</v>
       </c>
     </row>
@@ -2216,26 +2253,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16C6AB9-8B80-425A-BD7D-82836A637DC5}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -2250,12 +2288,15 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.7813596629142801</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <f>1/A2*10000</f>
         <v>2091.4552982832743</v>
       </c>
@@ -2274,12 +2315,16 @@
         <f>EXP(26.5-45210/B2)</f>
         <v>132.08860718813861</v>
       </c>
+      <c r="G2">
+        <f>10^(11.5-19630/B2)</f>
+        <v>130.07414554362003</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5.0217623330069001</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <f t="shared" ref="B3:B7" si="0">1/A3*10000</f>
         <v>1991.3327905369549</v>
       </c>
@@ -2298,12 +2343,16 @@
         <f t="shared" ref="F3:F7" si="3">EXP(26.5-45210/B3)</f>
         <v>44.550015082805274</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="4">10^(11.5-19630/B3)</f>
+        <v>43.881406605559583</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.2843738489043801</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>1892.3717900983331</v>
       </c>
@@ -2322,12 +2371,16 @@
         <f t="shared" si="3"/>
         <v>13.590157657692417</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>13.389801371532043</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.5731157968501499</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>1794.3284088322489</v>
       </c>
@@ -2346,12 +2399,16 @@
         <f t="shared" si="3"/>
         <v>3.6837950428522164</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>3.6305606045439478</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.89974395141365</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>1694.9888134728083</v>
       </c>
@@ -2370,12 +2427,16 @@
         <f t="shared" si="3"/>
         <v>0.84135431615219503</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>0.82947370555269306</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6.2211478163996796</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>1607.4204142262654</v>
       </c>
@@ -2393,6 +2454,10 @@
       <c r="F7">
         <f t="shared" si="3"/>
         <v>0.19675238339310983</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0.19403802091697159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>